<commit_message>
Adjusted Verification for CoolTerm for teachinglab-four bar
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/Experimental/CoolTerm/f10_2RPM.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/Experimental/CoolTerm/f10_2RPM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\TeachingLab_Four_Bar\Experimental\CoolTerm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E62E51C-077B-4842-BAB6-86EC74891227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EA5EFC7-14C1-4600-8A22-FCAFE0D8A0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12096" tabRatio="500" xr2:uid="{8E086815-7F18-4EFE-BA2A-02D39BCF37D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12096" tabRatio="500" xr2:uid="{841305C8-7A9F-47AF-8AED-1298C162DFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sep 4 Trial" sheetId="1" r:id="rId1"/>
@@ -226,35 +226,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -282,6 +256,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -682,11 +680,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97265641-9848-488D-8E78-E1250C20A192}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5204AB0D-8214-4A3A-AF95-F93C6374BC9A}">
   <dimension ref="A1:S342"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -704,121 +702,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="18" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="20"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="10"/>
     </row>
     <row r="2" spans="1:19" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="3" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="1" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="1" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="1" t="s">
+      <c r="O2" s="14"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="7"/>
-      <c r="S2" s="8"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="1:19" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="4" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -886,7 +884,7 @@
       <c r="A5">
         <v>68421</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <f t="shared" ref="B5:B68" si="0">A5-$A$4</f>
         <v>106</v>
       </c>
@@ -946,7 +944,7 @@
       <c r="A6">
         <v>68529</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>214</v>
       </c>
@@ -1006,7 +1004,7 @@
       <c r="A7">
         <v>68636</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>321</v>
       </c>
@@ -1066,7 +1064,7 @@
       <c r="A8">
         <v>68744</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>429</v>
       </c>
@@ -1126,7 +1124,7 @@
       <c r="A9">
         <v>68850</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>535</v>
       </c>
@@ -1186,7 +1184,7 @@
       <c r="A10">
         <v>68956</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>641</v>
       </c>
@@ -1246,7 +1244,7 @@
       <c r="A11">
         <v>69061</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <f t="shared" si="0"/>
         <v>746</v>
       </c>
@@ -1306,7 +1304,7 @@
       <c r="A12">
         <v>69165</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <f t="shared" si="0"/>
         <v>850</v>
       </c>
@@ -1362,63 +1360,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>69269</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13">
         <f t="shared" si="0"/>
         <v>954</v>
       </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>-0.54</v>
       </c>
-      <c r="E13" s="6">
-        <v>0.12</v>
-      </c>
-      <c r="F13" s="6">
+      <c r="E13">
+        <v>0.12</v>
+      </c>
+      <c r="F13">
         <v>9.17</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13">
         <v>0.25</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13">
         <v>0.75</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13">
         <v>0.06</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13">
         <v>3.19</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L13" s="6">
-        <v>0</v>
-      </c>
-      <c r="M13" s="6">
-        <v>0</v>
-      </c>
-      <c r="N13" s="6">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
         <v>359.94</v>
       </c>
-      <c r="O13" s="6">
-        <v>0.12</v>
-      </c>
-      <c r="P13" s="6">
+      <c r="O13">
+        <v>0.12</v>
+      </c>
+      <c r="P13">
         <v>-6.19</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13">
         <v>0.56999999999999995</v>
       </c>
-      <c r="R13" s="6">
-        <v>0</v>
-      </c>
-      <c r="S13" s="6">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
         <v>-0.01</v>
       </c>
     </row>
@@ -1426,7 +1424,7 @@
       <c r="A14">
         <v>69372</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <f t="shared" si="0"/>
         <v>1057</v>
       </c>
@@ -1486,7 +1484,7 @@
       <c r="A15">
         <v>69479</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <f t="shared" si="0"/>
         <v>1164</v>
       </c>
@@ -1546,7 +1544,7 @@
       <c r="A16">
         <v>69584</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <f t="shared" si="0"/>
         <v>1269</v>
       </c>
@@ -1606,7 +1604,7 @@
       <c r="A17">
         <v>69692</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <f t="shared" si="0"/>
         <v>1377</v>
       </c>
@@ -1666,7 +1664,7 @@
       <c r="A18">
         <v>69798</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <f t="shared" si="0"/>
         <v>1483</v>
       </c>
@@ -1726,7 +1724,7 @@
       <c r="A19">
         <v>69904</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <f t="shared" si="0"/>
         <v>1589</v>
       </c>
@@ -1786,7 +1784,7 @@
       <c r="A20">
         <v>70012</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <f t="shared" si="0"/>
         <v>1697</v>
       </c>
@@ -1846,7 +1844,7 @@
       <c r="A21">
         <v>70120</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <f t="shared" si="0"/>
         <v>1805</v>
       </c>
@@ -1906,7 +1904,7 @@
       <c r="A22">
         <v>70227</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <f t="shared" si="0"/>
         <v>1912</v>
       </c>
@@ -1966,7 +1964,7 @@
       <c r="A23">
         <v>70336</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
@@ -2026,7 +2024,7 @@
       <c r="A24">
         <v>70444</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <f t="shared" si="0"/>
         <v>2129</v>
       </c>
@@ -2086,7 +2084,7 @@
       <c r="A25">
         <v>70551</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25">
         <f t="shared" si="0"/>
         <v>2236</v>
       </c>
@@ -2146,7 +2144,7 @@
       <c r="A26">
         <v>70658</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26">
         <f t="shared" si="0"/>
         <v>2343</v>
       </c>
@@ -2206,7 +2204,7 @@
       <c r="A27">
         <v>70764</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27">
         <f t="shared" si="0"/>
         <v>2449</v>
       </c>
@@ -2266,7 +2264,7 @@
       <c r="A28">
         <v>70872</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28">
         <f t="shared" si="0"/>
         <v>2557</v>
       </c>
@@ -2326,7 +2324,7 @@
       <c r="A29">
         <v>70977</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29">
         <f t="shared" si="0"/>
         <v>2662</v>
       </c>
@@ -2386,7 +2384,7 @@
       <c r="A30">
         <v>71085</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30">
         <f t="shared" si="0"/>
         <v>2770</v>
       </c>
@@ -2446,7 +2444,7 @@
       <c r="A31">
         <v>71192</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31">
         <f t="shared" si="0"/>
         <v>2877</v>
       </c>
@@ -2506,7 +2504,7 @@
       <c r="A32">
         <v>71300</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32">
         <f t="shared" si="0"/>
         <v>2985</v>
       </c>
@@ -2566,7 +2564,7 @@
       <c r="A33">
         <v>71408</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33">
         <f t="shared" si="0"/>
         <v>3093</v>
       </c>
@@ -2626,7 +2624,7 @@
       <c r="A34">
         <v>71516</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34">
         <f t="shared" si="0"/>
         <v>3201</v>
       </c>
@@ -2686,7 +2684,7 @@
       <c r="A35">
         <v>71624</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35">
         <f t="shared" si="0"/>
         <v>3309</v>
       </c>
@@ -2746,7 +2744,7 @@
       <c r="A36">
         <v>71731</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36">
         <f t="shared" si="0"/>
         <v>3416</v>
       </c>
@@ -2806,7 +2804,7 @@
       <c r="A37">
         <v>71836</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37">
         <f t="shared" si="0"/>
         <v>3521</v>
       </c>
@@ -2866,7 +2864,7 @@
       <c r="A38">
         <v>71942</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38">
         <f t="shared" si="0"/>
         <v>3627</v>
       </c>
@@ -2926,7 +2924,7 @@
       <c r="A39">
         <v>72047</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39">
         <f t="shared" si="0"/>
         <v>3732</v>
       </c>
@@ -2986,7 +2984,7 @@
       <c r="A40">
         <v>72154</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40">
         <f t="shared" si="0"/>
         <v>3839</v>
       </c>
@@ -3046,7 +3044,7 @@
       <c r="A41">
         <v>72261</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41">
         <f t="shared" si="0"/>
         <v>3946</v>
       </c>
@@ -3106,7 +3104,7 @@
       <c r="A42">
         <v>72367</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42">
         <f t="shared" si="0"/>
         <v>4052</v>
       </c>
@@ -3166,7 +3164,7 @@
       <c r="A43">
         <v>72474</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43">
         <f t="shared" si="0"/>
         <v>4159</v>
       </c>
@@ -3226,7 +3224,7 @@
       <c r="A44">
         <v>72580</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44">
         <f t="shared" si="0"/>
         <v>4265</v>
       </c>
@@ -3286,7 +3284,7 @@
       <c r="A45">
         <v>72687</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45">
         <f t="shared" si="0"/>
         <v>4372</v>
       </c>
@@ -3346,7 +3344,7 @@
       <c r="A46">
         <v>72794</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46">
         <f t="shared" si="0"/>
         <v>4479</v>
       </c>
@@ -3406,7 +3404,7 @@
       <c r="A47">
         <v>72899</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47">
         <f t="shared" si="0"/>
         <v>4584</v>
       </c>
@@ -3466,7 +3464,7 @@
       <c r="A48">
         <v>73006</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48">
         <f t="shared" si="0"/>
         <v>4691</v>
       </c>
@@ -3526,7 +3524,7 @@
       <c r="A49">
         <v>73110</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49">
         <f t="shared" si="0"/>
         <v>4795</v>
       </c>
@@ -3586,7 +3584,7 @@
       <c r="A50">
         <v>73213</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50">
         <f t="shared" si="0"/>
         <v>4898</v>
       </c>
@@ -3646,7 +3644,7 @@
       <c r="A51">
         <v>73317</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51">
         <f t="shared" si="0"/>
         <v>5002</v>
       </c>
@@ -3706,7 +3704,7 @@
       <c r="A52">
         <v>73420</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52">
         <f t="shared" si="0"/>
         <v>5105</v>
       </c>
@@ -3766,7 +3764,7 @@
       <c r="A53">
         <v>73525</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53">
         <f t="shared" si="0"/>
         <v>5210</v>
       </c>
@@ -3826,7 +3824,7 @@
       <c r="A54">
         <v>73628</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54">
         <f t="shared" si="0"/>
         <v>5313</v>
       </c>
@@ -3886,7 +3884,7 @@
       <c r="A55">
         <v>73735</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55">
         <f t="shared" si="0"/>
         <v>5420</v>
       </c>
@@ -3946,7 +3944,7 @@
       <c r="A56">
         <v>73840</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56">
         <f t="shared" si="0"/>
         <v>5525</v>
       </c>
@@ -4006,7 +4004,7 @@
       <c r="A57">
         <v>73946</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57">
         <f t="shared" si="0"/>
         <v>5631</v>
       </c>
@@ -4066,7 +4064,7 @@
       <c r="A58">
         <v>74050</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58">
         <f t="shared" si="0"/>
         <v>5735</v>
       </c>
@@ -4126,7 +4124,7 @@
       <c r="A59">
         <v>74157</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59">
         <f t="shared" si="0"/>
         <v>5842</v>
       </c>
@@ -4186,7 +4184,7 @@
       <c r="A60">
         <v>74263</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60">
         <f t="shared" si="0"/>
         <v>5948</v>
       </c>
@@ -4246,7 +4244,7 @@
       <c r="A61">
         <v>74370</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61">
         <f t="shared" si="0"/>
         <v>6055</v>
       </c>
@@ -4306,7 +4304,7 @@
       <c r="A62">
         <v>74478</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62">
         <f t="shared" si="0"/>
         <v>6163</v>
       </c>
@@ -4366,7 +4364,7 @@
       <c r="A63">
         <v>74586</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63">
         <f t="shared" si="0"/>
         <v>6271</v>
       </c>
@@ -4426,7 +4424,7 @@
       <c r="A64">
         <v>74693</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64">
         <f t="shared" si="0"/>
         <v>6378</v>
       </c>
@@ -4486,7 +4484,7 @@
       <c r="A65">
         <v>74799</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65">
         <f t="shared" si="0"/>
         <v>6484</v>
       </c>
@@ -4546,7 +4544,7 @@
       <c r="A66">
         <v>74904</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66">
         <f t="shared" si="0"/>
         <v>6589</v>
       </c>
@@ -4602,63 +4600,63 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="67" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>75009</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67">
         <f t="shared" si="0"/>
         <v>6694</v>
       </c>
-      <c r="C67" s="6">
-        <v>0</v>
-      </c>
-      <c r="D67" s="6">
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="E67" s="6">
+      <c r="E67">
         <v>0.02</v>
       </c>
-      <c r="F67" s="6">
+      <c r="F67">
         <v>7.85</v>
       </c>
-      <c r="G67" s="6">
+      <c r="G67">
         <v>0.15</v>
       </c>
-      <c r="H67" s="6">
+      <c r="H67">
         <v>0.88</v>
       </c>
-      <c r="I67" s="6">
+      <c r="I67">
         <v>0.06</v>
       </c>
-      <c r="J67" s="6">
+      <c r="J67">
         <v>4.4400000000000004</v>
       </c>
-      <c r="K67" s="6">
+      <c r="K67">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L67" s="6">
+      <c r="L67">
         <v>-0.01</v>
       </c>
-      <c r="M67" s="6">
-        <v>0</v>
-      </c>
-      <c r="N67" s="6">
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67">
         <v>359.94</v>
       </c>
-      <c r="O67" s="6">
-        <v>0.12</v>
-      </c>
-      <c r="P67" s="6">
+      <c r="O67">
+        <v>0.12</v>
+      </c>
+      <c r="P67">
         <v>-4.63</v>
       </c>
-      <c r="Q67" s="6">
+      <c r="Q67">
         <v>0.63</v>
       </c>
-      <c r="R67" s="6">
-        <v>0</v>
-      </c>
-      <c r="S67" s="6">
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67">
         <v>-0.01</v>
       </c>
     </row>
@@ -4666,7 +4664,7 @@
       <c r="A68">
         <v>75112</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68">
         <f t="shared" si="0"/>
         <v>6797</v>
       </c>
@@ -4726,7 +4724,7 @@
       <c r="A69">
         <v>75217</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69">
         <f t="shared" ref="B69:B132" si="1">A69-$A$4</f>
         <v>6902</v>
       </c>
@@ -4786,7 +4784,7 @@
       <c r="A70">
         <v>75326</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70">
         <f t="shared" si="1"/>
         <v>7011</v>
       </c>
@@ -4846,7 +4844,7 @@
       <c r="A71">
         <v>75432</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71">
         <f t="shared" si="1"/>
         <v>7117</v>
       </c>
@@ -4906,7 +4904,7 @@
       <c r="A72">
         <v>75540</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72">
         <f t="shared" si="1"/>
         <v>7225</v>
       </c>
@@ -4966,7 +4964,7 @@
       <c r="A73">
         <v>75649</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73">
         <f t="shared" si="1"/>
         <v>7334</v>
       </c>
@@ -5026,7 +5024,7 @@
       <c r="A74">
         <v>75758</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74">
         <f t="shared" si="1"/>
         <v>7443</v>
       </c>
@@ -5086,7 +5084,7 @@
       <c r="A75">
         <v>75868</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75">
         <f t="shared" si="1"/>
         <v>7553</v>
       </c>
@@ -5146,7 +5144,7 @@
       <c r="A76">
         <v>75975</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76">
         <f t="shared" si="1"/>
         <v>7660</v>
       </c>
@@ -5206,7 +5204,7 @@
       <c r="A77">
         <v>76085</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77">
         <f t="shared" si="1"/>
         <v>7770</v>
       </c>
@@ -5266,7 +5264,7 @@
       <c r="A78">
         <v>76192</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78">
         <f t="shared" si="1"/>
         <v>7877</v>
       </c>
@@ -5326,7 +5324,7 @@
       <c r="A79">
         <v>76299</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79">
         <f t="shared" si="1"/>
         <v>7984</v>
       </c>
@@ -5386,7 +5384,7 @@
       <c r="A80">
         <v>76406</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80">
         <f t="shared" si="1"/>
         <v>8091</v>
       </c>
@@ -5446,7 +5444,7 @@
       <c r="A81">
         <v>76513</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81">
         <f t="shared" si="1"/>
         <v>8198</v>
       </c>
@@ -5506,7 +5504,7 @@
       <c r="A82">
         <v>76619</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82">
         <f t="shared" si="1"/>
         <v>8304</v>
       </c>
@@ -5566,7 +5564,7 @@
       <c r="A83">
         <v>76726</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83">
         <f t="shared" si="1"/>
         <v>8411</v>
       </c>
@@ -5626,7 +5624,7 @@
       <c r="A84">
         <v>76830</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84">
         <f t="shared" si="1"/>
         <v>8515</v>
       </c>
@@ -5686,7 +5684,7 @@
       <c r="A85">
         <v>76938</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85">
         <f t="shared" si="1"/>
         <v>8623</v>
       </c>
@@ -5746,7 +5744,7 @@
       <c r="A86">
         <v>77045</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86">
         <f t="shared" si="1"/>
         <v>8730</v>
       </c>
@@ -5806,7 +5804,7 @@
       <c r="A87">
         <v>77155</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87">
         <f t="shared" si="1"/>
         <v>8840</v>
       </c>
@@ -5866,7 +5864,7 @@
       <c r="A88">
         <v>77263</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88">
         <f t="shared" si="1"/>
         <v>8948</v>
       </c>
@@ -5926,7 +5924,7 @@
       <c r="A89">
         <v>77372</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89">
         <f t="shared" si="1"/>
         <v>9057</v>
       </c>
@@ -5986,7 +5984,7 @@
       <c r="A90">
         <v>77480</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90">
         <f t="shared" si="1"/>
         <v>9165</v>
       </c>
@@ -6046,7 +6044,7 @@
       <c r="A91">
         <v>77587</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91">
         <f t="shared" si="1"/>
         <v>9272</v>
       </c>
@@ -6106,7 +6104,7 @@
       <c r="A92">
         <v>77692</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92">
         <f t="shared" si="1"/>
         <v>9377</v>
       </c>
@@ -6166,7 +6164,7 @@
       <c r="A93">
         <v>77799</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93">
         <f t="shared" si="1"/>
         <v>9484</v>
       </c>
@@ -6226,7 +6224,7 @@
       <c r="A94">
         <v>77904</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94">
         <f t="shared" si="1"/>
         <v>9589</v>
       </c>
@@ -6286,7 +6284,7 @@
       <c r="A95">
         <v>78012</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95">
         <f t="shared" si="1"/>
         <v>9697</v>
       </c>
@@ -6346,7 +6344,7 @@
       <c r="A96">
         <v>78118</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96">
         <f t="shared" si="1"/>
         <v>9803</v>
       </c>
@@ -6406,7 +6404,7 @@
       <c r="A97">
         <v>78226</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97">
         <f t="shared" si="1"/>
         <v>9911</v>
       </c>
@@ -6466,7 +6464,7 @@
       <c r="A98">
         <v>78332</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98">
         <f t="shared" si="1"/>
         <v>10017</v>
       </c>
@@ -6526,7 +6524,7 @@
       <c r="A99">
         <v>78438</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99">
         <f t="shared" si="1"/>
         <v>10123</v>
       </c>
@@ -6586,7 +6584,7 @@
       <c r="A100">
         <v>78545</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100">
         <f t="shared" si="1"/>
         <v>10230</v>
       </c>
@@ -6646,7 +6644,7 @@
       <c r="A101">
         <v>78652</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101">
         <f t="shared" si="1"/>
         <v>10337</v>
       </c>
@@ -6706,7 +6704,7 @@
       <c r="A102">
         <v>78756</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B102">
         <f t="shared" si="1"/>
         <v>10441</v>
       </c>
@@ -6766,7 +6764,7 @@
       <c r="A103">
         <v>78862</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B103">
         <f t="shared" si="1"/>
         <v>10547</v>
       </c>
@@ -6826,7 +6824,7 @@
       <c r="A104">
         <v>78965</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B104">
         <f t="shared" si="1"/>
         <v>10650</v>
       </c>
@@ -6886,7 +6884,7 @@
       <c r="A105">
         <v>79069</v>
       </c>
-      <c r="B105" s="2">
+      <c r="B105">
         <f t="shared" si="1"/>
         <v>10754</v>
       </c>
@@ -6946,7 +6944,7 @@
       <c r="A106">
         <v>79171</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B106">
         <f t="shared" si="1"/>
         <v>10856</v>
       </c>
@@ -7006,7 +7004,7 @@
       <c r="A107">
         <v>79273</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B107">
         <f t="shared" si="1"/>
         <v>10958</v>
       </c>
@@ -7066,7 +7064,7 @@
       <c r="A108">
         <v>79377</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B108">
         <f t="shared" si="1"/>
         <v>11062</v>
       </c>
@@ -7126,7 +7124,7 @@
       <c r="A109">
         <v>79482</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B109">
         <f t="shared" si="1"/>
         <v>11167</v>
       </c>
@@ -7186,7 +7184,7 @@
       <c r="A110">
         <v>79588</v>
       </c>
-      <c r="B110" s="2">
+      <c r="B110">
         <f t="shared" si="1"/>
         <v>11273</v>
       </c>
@@ -7246,7 +7244,7 @@
       <c r="A111">
         <v>79691</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B111">
         <f t="shared" si="1"/>
         <v>11376</v>
       </c>
@@ -7306,7 +7304,7 @@
       <c r="A112">
         <v>79797</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B112">
         <f t="shared" si="1"/>
         <v>11482</v>
       </c>
@@ -7366,7 +7364,7 @@
       <c r="A113">
         <v>79901</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113">
         <f t="shared" si="1"/>
         <v>11586</v>
       </c>
@@ -7426,7 +7424,7 @@
       <c r="A114">
         <v>80008</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B114">
         <f t="shared" si="1"/>
         <v>11693</v>
       </c>
@@ -7486,7 +7484,7 @@
       <c r="A115">
         <v>80116</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B115">
         <f t="shared" si="1"/>
         <v>11801</v>
       </c>
@@ -7546,7 +7544,7 @@
       <c r="A116">
         <v>80223</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B116">
         <f t="shared" si="1"/>
         <v>11908</v>
       </c>
@@ -7606,7 +7604,7 @@
       <c r="A117">
         <v>80328</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B117">
         <f t="shared" si="1"/>
         <v>12013</v>
       </c>
@@ -7666,7 +7664,7 @@
       <c r="A118">
         <v>80434</v>
       </c>
-      <c r="B118" s="2">
+      <c r="B118">
         <f t="shared" si="1"/>
         <v>12119</v>
       </c>
@@ -7726,7 +7724,7 @@
       <c r="A119">
         <v>80539</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B119">
         <f t="shared" si="1"/>
         <v>12224</v>
       </c>
@@ -7786,7 +7784,7 @@
       <c r="A120">
         <v>80644</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B120">
         <f t="shared" si="1"/>
         <v>12329</v>
       </c>
@@ -7846,7 +7844,7 @@
       <c r="A121">
         <v>80747</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B121">
         <f t="shared" si="1"/>
         <v>12432</v>
       </c>
@@ -7906,7 +7904,7 @@
       <c r="A122">
         <v>80851</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B122">
         <f t="shared" si="1"/>
         <v>12536</v>
       </c>
@@ -7966,7 +7964,7 @@
       <c r="A123">
         <v>80953</v>
       </c>
-      <c r="B123" s="2">
+      <c r="B123">
         <f t="shared" si="1"/>
         <v>12638</v>
       </c>
@@ -8026,7 +8024,7 @@
       <c r="A124">
         <v>81059</v>
       </c>
-      <c r="B124" s="2">
+      <c r="B124">
         <f t="shared" si="1"/>
         <v>12744</v>
       </c>
@@ -8086,7 +8084,7 @@
       <c r="A125">
         <v>81167</v>
       </c>
-      <c r="B125" s="2">
+      <c r="B125">
         <f t="shared" si="1"/>
         <v>12852</v>
       </c>
@@ -8146,7 +8144,7 @@
       <c r="A126">
         <v>81274</v>
       </c>
-      <c r="B126" s="2">
+      <c r="B126">
         <f t="shared" si="1"/>
         <v>12959</v>
       </c>
@@ -8206,7 +8204,7 @@
       <c r="A127">
         <v>81381</v>
       </c>
-      <c r="B127" s="2">
+      <c r="B127">
         <f t="shared" si="1"/>
         <v>13066</v>
       </c>
@@ -8266,7 +8264,7 @@
       <c r="A128">
         <v>81486</v>
       </c>
-      <c r="B128" s="2">
+      <c r="B128">
         <f t="shared" si="1"/>
         <v>13171</v>
       </c>
@@ -8326,7 +8324,7 @@
       <c r="A129">
         <v>81595</v>
       </c>
-      <c r="B129" s="2">
+      <c r="B129">
         <f t="shared" si="1"/>
         <v>13280</v>
       </c>
@@ -8386,7 +8384,7 @@
       <c r="A130">
         <v>81702</v>
       </c>
-      <c r="B130" s="2">
+      <c r="B130">
         <f t="shared" si="1"/>
         <v>13387</v>
       </c>
@@ -8446,7 +8444,7 @@
       <c r="A131">
         <v>81811</v>
       </c>
-      <c r="B131" s="2">
+      <c r="B131">
         <f t="shared" si="1"/>
         <v>13496</v>
       </c>
@@ -8506,7 +8504,7 @@
       <c r="A132">
         <v>81918</v>
       </c>
-      <c r="B132" s="2">
+      <c r="B132">
         <f t="shared" si="1"/>
         <v>13603</v>
       </c>
@@ -8566,7 +8564,7 @@
       <c r="A133">
         <v>82024</v>
       </c>
-      <c r="B133" s="2">
+      <c r="B133">
         <f t="shared" ref="B133:B196" si="2">A133-$A$4</f>
         <v>13709</v>
       </c>
@@ -8626,7 +8624,7 @@
       <c r="A134">
         <v>82130</v>
       </c>
-      <c r="B134" s="2">
+      <c r="B134">
         <f t="shared" si="2"/>
         <v>13815</v>
       </c>
@@ -8686,7 +8684,7 @@
       <c r="A135">
         <v>82236</v>
       </c>
-      <c r="B135" s="2">
+      <c r="B135">
         <f t="shared" si="2"/>
         <v>13921</v>
       </c>
@@ -8746,7 +8744,7 @@
       <c r="A136">
         <v>82341</v>
       </c>
-      <c r="B136" s="2">
+      <c r="B136">
         <f t="shared" si="2"/>
         <v>14026</v>
       </c>
@@ -8806,7 +8804,7 @@
       <c r="A137">
         <v>82448</v>
       </c>
-      <c r="B137" s="2">
+      <c r="B137">
         <f t="shared" si="2"/>
         <v>14133</v>
       </c>
@@ -8866,7 +8864,7 @@
       <c r="A138">
         <v>82553</v>
       </c>
-      <c r="B138" s="2">
+      <c r="B138">
         <f t="shared" si="2"/>
         <v>14238</v>
       </c>
@@ -8926,7 +8924,7 @@
       <c r="A139">
         <v>82660</v>
       </c>
-      <c r="B139" s="2">
+      <c r="B139">
         <f t="shared" si="2"/>
         <v>14345</v>
       </c>
@@ -8986,7 +8984,7 @@
       <c r="A140">
         <v>82766</v>
       </c>
-      <c r="B140" s="2">
+      <c r="B140">
         <f t="shared" si="2"/>
         <v>14451</v>
       </c>
@@ -9046,7 +9044,7 @@
       <c r="A141">
         <v>82873</v>
       </c>
-      <c r="B141" s="2">
+      <c r="B141">
         <f t="shared" si="2"/>
         <v>14558</v>
       </c>
@@ -9106,7 +9104,7 @@
       <c r="A142">
         <v>82980</v>
       </c>
-      <c r="B142" s="2">
+      <c r="B142">
         <f t="shared" si="2"/>
         <v>14665</v>
       </c>
@@ -9166,7 +9164,7 @@
       <c r="A143">
         <v>83087</v>
       </c>
-      <c r="B143" s="2">
+      <c r="B143">
         <f t="shared" si="2"/>
         <v>14772</v>
       </c>
@@ -9226,7 +9224,7 @@
       <c r="A144">
         <v>83194</v>
       </c>
-      <c r="B144" s="2">
+      <c r="B144">
         <f t="shared" si="2"/>
         <v>14879</v>
       </c>
@@ -9286,7 +9284,7 @@
       <c r="A145">
         <v>83300</v>
       </c>
-      <c r="B145" s="2">
+      <c r="B145">
         <f t="shared" si="2"/>
         <v>14985</v>
       </c>
@@ -9346,7 +9344,7 @@
       <c r="A146">
         <v>83405</v>
       </c>
-      <c r="B146" s="2">
+      <c r="B146">
         <f t="shared" si="2"/>
         <v>15090</v>
       </c>
@@ -9406,7 +9404,7 @@
       <c r="A147">
         <v>83510</v>
       </c>
-      <c r="B147" s="2">
+      <c r="B147">
         <f t="shared" si="2"/>
         <v>15195</v>
       </c>
@@ -9466,7 +9464,7 @@
       <c r="A148">
         <v>83614</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B148">
         <f t="shared" si="2"/>
         <v>15299</v>
       </c>
@@ -9526,7 +9524,7 @@
       <c r="A149">
         <v>83721</v>
       </c>
-      <c r="B149" s="2">
+      <c r="B149">
         <f t="shared" si="2"/>
         <v>15406</v>
       </c>
@@ -9586,7 +9584,7 @@
       <c r="A150">
         <v>83827</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B150">
         <f t="shared" si="2"/>
         <v>15512</v>
       </c>
@@ -9646,7 +9644,7 @@
       <c r="A151">
         <v>83933</v>
       </c>
-      <c r="B151" s="2">
+      <c r="B151">
         <f t="shared" si="2"/>
         <v>15618</v>
       </c>
@@ -9706,7 +9704,7 @@
       <c r="A152">
         <v>84038</v>
       </c>
-      <c r="B152" s="2">
+      <c r="B152">
         <f t="shared" si="2"/>
         <v>15723</v>
       </c>
@@ -9766,7 +9764,7 @@
       <c r="A153">
         <v>84144</v>
       </c>
-      <c r="B153" s="2">
+      <c r="B153">
         <f t="shared" si="2"/>
         <v>15829</v>
       </c>
@@ -9826,7 +9824,7 @@
       <c r="A154">
         <v>84250</v>
       </c>
-      <c r="B154" s="2">
+      <c r="B154">
         <f t="shared" si="2"/>
         <v>15935</v>
       </c>
@@ -9886,7 +9884,7 @@
       <c r="A155">
         <v>84357</v>
       </c>
-      <c r="B155" s="2">
+      <c r="B155">
         <f t="shared" si="2"/>
         <v>16042</v>
       </c>
@@ -9946,7 +9944,7 @@
       <c r="A156">
         <v>84463</v>
       </c>
-      <c r="B156" s="2">
+      <c r="B156">
         <f t="shared" si="2"/>
         <v>16148</v>
       </c>
@@ -10006,7 +10004,7 @@
       <c r="A157">
         <v>84566</v>
       </c>
-      <c r="B157" s="2">
+      <c r="B157">
         <f t="shared" si="2"/>
         <v>16251</v>
       </c>
@@ -10066,7 +10064,7 @@
       <c r="A158">
         <v>84670</v>
       </c>
-      <c r="B158" s="2">
+      <c r="B158">
         <f t="shared" si="2"/>
         <v>16355</v>
       </c>
@@ -10126,7 +10124,7 @@
       <c r="A159">
         <v>84769</v>
       </c>
-      <c r="B159" s="2">
+      <c r="B159">
         <f t="shared" si="2"/>
         <v>16454</v>
       </c>
@@ -10186,7 +10184,7 @@
       <c r="A160">
         <v>84872</v>
       </c>
-      <c r="B160" s="2">
+      <c r="B160">
         <f t="shared" si="2"/>
         <v>16557</v>
       </c>
@@ -10246,7 +10244,7 @@
       <c r="A161">
         <v>84973</v>
       </c>
-      <c r="B161" s="2">
+      <c r="B161">
         <f t="shared" si="2"/>
         <v>16658</v>
       </c>
@@ -10306,7 +10304,7 @@
       <c r="A162">
         <v>85073</v>
       </c>
-      <c r="B162" s="2">
+      <c r="B162">
         <f t="shared" si="2"/>
         <v>16758</v>
       </c>
@@ -10366,7 +10364,7 @@
       <c r="A163">
         <v>85176</v>
       </c>
-      <c r="B163" s="2">
+      <c r="B163">
         <f t="shared" si="2"/>
         <v>16861</v>
       </c>
@@ -10426,7 +10424,7 @@
       <c r="A164">
         <v>85278</v>
       </c>
-      <c r="B164" s="2">
+      <c r="B164">
         <f t="shared" si="2"/>
         <v>16963</v>
       </c>
@@ -10486,7 +10484,7 @@
       <c r="A165">
         <v>85383</v>
       </c>
-      <c r="B165" s="2">
+      <c r="B165">
         <f t="shared" si="2"/>
         <v>17068</v>
       </c>
@@ -10546,7 +10544,7 @@
       <c r="A166">
         <v>85486</v>
       </c>
-      <c r="B166" s="2">
+      <c r="B166">
         <f t="shared" si="2"/>
         <v>17171</v>
       </c>
@@ -10606,7 +10604,7 @@
       <c r="A167">
         <v>85591</v>
       </c>
-      <c r="B167" s="2">
+      <c r="B167">
         <f t="shared" si="2"/>
         <v>17276</v>
       </c>
@@ -10666,7 +10664,7 @@
       <c r="A168">
         <v>85696</v>
       </c>
-      <c r="B168" s="2">
+      <c r="B168">
         <f t="shared" si="2"/>
         <v>17381</v>
       </c>
@@ -10726,7 +10724,7 @@
       <c r="A169">
         <v>85801</v>
       </c>
-      <c r="B169" s="2">
+      <c r="B169">
         <f t="shared" si="2"/>
         <v>17486</v>
       </c>
@@ -10786,7 +10784,7 @@
       <c r="A170">
         <v>85908</v>
       </c>
-      <c r="B170" s="2">
+      <c r="B170">
         <f t="shared" si="2"/>
         <v>17593</v>
       </c>
@@ -10846,7 +10844,7 @@
       <c r="A171">
         <v>86013</v>
       </c>
-      <c r="B171" s="2">
+      <c r="B171">
         <f t="shared" si="2"/>
         <v>17698</v>
       </c>
@@ -10906,7 +10904,7 @@
       <c r="A172">
         <v>86120</v>
       </c>
-      <c r="B172" s="2">
+      <c r="B172">
         <f t="shared" si="2"/>
         <v>17805</v>
       </c>
@@ -10966,7 +10964,7 @@
       <c r="A173">
         <v>86225</v>
       </c>
-      <c r="B173" s="2">
+      <c r="B173">
         <f t="shared" si="2"/>
         <v>17910</v>
       </c>
@@ -11026,7 +11024,7 @@
       <c r="A174">
         <v>86331</v>
       </c>
-      <c r="B174" s="2">
+      <c r="B174">
         <f t="shared" si="2"/>
         <v>18016</v>
       </c>
@@ -11086,7 +11084,7 @@
       <c r="A175">
         <v>86435</v>
       </c>
-      <c r="B175" s="2">
+      <c r="B175">
         <f t="shared" si="2"/>
         <v>18120</v>
       </c>
@@ -11146,7 +11144,7 @@
       <c r="A176">
         <v>86538</v>
       </c>
-      <c r="B176" s="2">
+      <c r="B176">
         <f t="shared" si="2"/>
         <v>18223</v>
       </c>
@@ -11206,7 +11204,7 @@
       <c r="A177">
         <v>86643</v>
       </c>
-      <c r="B177" s="2">
+      <c r="B177">
         <f t="shared" si="2"/>
         <v>18328</v>
       </c>
@@ -11266,7 +11264,7 @@
       <c r="A178">
         <v>86747</v>
       </c>
-      <c r="B178" s="2">
+      <c r="B178">
         <f t="shared" si="2"/>
         <v>18432</v>
       </c>
@@ -11326,7 +11324,7 @@
       <c r="A179">
         <v>86854</v>
       </c>
-      <c r="B179" s="2">
+      <c r="B179">
         <f t="shared" si="2"/>
         <v>18539</v>
       </c>
@@ -11386,7 +11384,7 @@
       <c r="A180">
         <v>86960</v>
       </c>
-      <c r="B180" s="2">
+      <c r="B180">
         <f t="shared" si="2"/>
         <v>18645</v>
       </c>
@@ -11446,7 +11444,7 @@
       <c r="A181">
         <v>87067</v>
       </c>
-      <c r="B181" s="2">
+      <c r="B181">
         <f t="shared" si="2"/>
         <v>18752</v>
       </c>
@@ -11506,7 +11504,7 @@
       <c r="A182">
         <v>87175</v>
       </c>
-      <c r="B182" s="2">
+      <c r="B182">
         <f t="shared" si="2"/>
         <v>18860</v>
       </c>
@@ -11566,7 +11564,7 @@
       <c r="A183">
         <v>87281</v>
       </c>
-      <c r="B183" s="2">
+      <c r="B183">
         <f t="shared" si="2"/>
         <v>18966</v>
       </c>
@@ -11626,7 +11624,7 @@
       <c r="A184">
         <v>87390</v>
       </c>
-      <c r="B184" s="2">
+      <c r="B184">
         <f t="shared" si="2"/>
         <v>19075</v>
       </c>
@@ -11686,7 +11684,7 @@
       <c r="A185">
         <v>87497</v>
       </c>
-      <c r="B185" s="2">
+      <c r="B185">
         <f t="shared" si="2"/>
         <v>19182</v>
       </c>
@@ -11746,7 +11744,7 @@
       <c r="A186">
         <v>87605</v>
       </c>
-      <c r="B186" s="2">
+      <c r="B186">
         <f t="shared" si="2"/>
         <v>19290</v>
       </c>
@@ -11806,7 +11804,7 @@
       <c r="A187">
         <v>87712</v>
       </c>
-      <c r="B187" s="2">
+      <c r="B187">
         <f t="shared" si="2"/>
         <v>19397</v>
       </c>
@@ -11866,7 +11864,7 @@
       <c r="A188">
         <v>87819</v>
       </c>
-      <c r="B188" s="2">
+      <c r="B188">
         <f t="shared" si="2"/>
         <v>19504</v>
       </c>
@@ -11926,7 +11924,7 @@
       <c r="A189">
         <v>87925</v>
       </c>
-      <c r="B189" s="2">
+      <c r="B189">
         <f t="shared" si="2"/>
         <v>19610</v>
       </c>
@@ -11986,7 +11984,7 @@
       <c r="A190">
         <v>88031</v>
       </c>
-      <c r="B190" s="2">
+      <c r="B190">
         <f t="shared" si="2"/>
         <v>19716</v>
       </c>
@@ -12046,7 +12044,7 @@
       <c r="A191">
         <v>88136</v>
       </c>
-      <c r="B191" s="2">
+      <c r="B191">
         <f t="shared" si="2"/>
         <v>19821</v>
       </c>
@@ -12106,7 +12104,7 @@
       <c r="A192">
         <v>88243</v>
       </c>
-      <c r="B192" s="2">
+      <c r="B192">
         <f t="shared" si="2"/>
         <v>19928</v>
       </c>
@@ -12166,7 +12164,7 @@
       <c r="A193">
         <v>88348</v>
       </c>
-      <c r="B193" s="2">
+      <c r="B193">
         <f t="shared" si="2"/>
         <v>20033</v>
       </c>
@@ -12226,7 +12224,7 @@
       <c r="A194">
         <v>88456</v>
       </c>
-      <c r="B194" s="2">
+      <c r="B194">
         <f t="shared" si="2"/>
         <v>20141</v>
       </c>
@@ -12286,7 +12284,7 @@
       <c r="A195">
         <v>88563</v>
       </c>
-      <c r="B195" s="2">
+      <c r="B195">
         <f t="shared" si="2"/>
         <v>20248</v>
       </c>
@@ -12346,7 +12344,7 @@
       <c r="A196">
         <v>88671</v>
       </c>
-      <c r="B196" s="2">
+      <c r="B196">
         <f t="shared" si="2"/>
         <v>20356</v>
       </c>
@@ -12406,7 +12404,7 @@
       <c r="A197">
         <v>88778</v>
       </c>
-      <c r="B197" s="2">
+      <c r="B197">
         <f t="shared" ref="B197:B260" si="3">A197-$A$4</f>
         <v>20463</v>
       </c>
@@ -12466,7 +12464,7 @@
       <c r="A198">
         <v>88885</v>
       </c>
-      <c r="B198" s="2">
+      <c r="B198">
         <f t="shared" si="3"/>
         <v>20570</v>
       </c>
@@ -12526,7 +12524,7 @@
       <c r="A199">
         <v>88992</v>
       </c>
-      <c r="B199" s="2">
+      <c r="B199">
         <f t="shared" si="3"/>
         <v>20677</v>
       </c>
@@ -12586,7 +12584,7 @@
       <c r="A200">
         <v>89100</v>
       </c>
-      <c r="B200" s="2">
+      <c r="B200">
         <f t="shared" si="3"/>
         <v>20785</v>
       </c>
@@ -12646,7 +12644,7 @@
       <c r="A201">
         <v>89206</v>
       </c>
-      <c r="B201" s="2">
+      <c r="B201">
         <f t="shared" si="3"/>
         <v>20891</v>
       </c>
@@ -12706,7 +12704,7 @@
       <c r="A202">
         <v>89314</v>
       </c>
-      <c r="B202" s="2">
+      <c r="B202">
         <f t="shared" si="3"/>
         <v>20999</v>
       </c>
@@ -12766,7 +12764,7 @@
       <c r="A203">
         <v>89421</v>
       </c>
-      <c r="B203" s="2">
+      <c r="B203">
         <f t="shared" si="3"/>
         <v>21106</v>
       </c>
@@ -12826,7 +12824,7 @@
       <c r="A204">
         <v>89527</v>
       </c>
-      <c r="B204" s="2">
+      <c r="B204">
         <f t="shared" si="3"/>
         <v>21212</v>
       </c>
@@ -12886,7 +12884,7 @@
       <c r="A205">
         <v>89632</v>
       </c>
-      <c r="B205" s="2">
+      <c r="B205">
         <f t="shared" si="3"/>
         <v>21317</v>
       </c>
@@ -12946,7 +12944,7 @@
       <c r="A206">
         <v>89736</v>
       </c>
-      <c r="B206" s="2">
+      <c r="B206">
         <f t="shared" si="3"/>
         <v>21421</v>
       </c>
@@ -13006,7 +13004,7 @@
       <c r="A207">
         <v>89842</v>
       </c>
-      <c r="B207" s="2">
+      <c r="B207">
         <f t="shared" si="3"/>
         <v>21527</v>
       </c>
@@ -13066,7 +13064,7 @@
       <c r="A208">
         <v>89947</v>
       </c>
-      <c r="B208" s="2">
+      <c r="B208">
         <f t="shared" si="3"/>
         <v>21632</v>
       </c>
@@ -13126,7 +13124,7 @@
       <c r="A209">
         <v>90053</v>
       </c>
-      <c r="B209" s="2">
+      <c r="B209">
         <f t="shared" si="3"/>
         <v>21738</v>
       </c>
@@ -13186,7 +13184,7 @@
       <c r="A210">
         <v>90159</v>
       </c>
-      <c r="B210" s="2">
+      <c r="B210">
         <f t="shared" si="3"/>
         <v>21844</v>
       </c>
@@ -13246,7 +13244,7 @@
       <c r="A211">
         <v>90264</v>
       </c>
-      <c r="B211" s="2">
+      <c r="B211">
         <f t="shared" si="3"/>
         <v>21949</v>
       </c>
@@ -13306,7 +13304,7 @@
       <c r="A212">
         <v>90369</v>
       </c>
-      <c r="B212" s="2">
+      <c r="B212">
         <f t="shared" si="3"/>
         <v>22054</v>
       </c>
@@ -13366,7 +13364,7 @@
       <c r="A213">
         <v>90470</v>
       </c>
-      <c r="B213" s="2">
+      <c r="B213">
         <f t="shared" si="3"/>
         <v>22155</v>
       </c>
@@ -13426,7 +13424,7 @@
       <c r="A214">
         <v>90573</v>
       </c>
-      <c r="B214" s="2">
+      <c r="B214">
         <f t="shared" si="3"/>
         <v>22258</v>
       </c>
@@ -13486,7 +13484,7 @@
       <c r="A215">
         <v>90674</v>
       </c>
-      <c r="B215" s="2">
+      <c r="B215">
         <f t="shared" si="3"/>
         <v>22359</v>
       </c>
@@ -13546,7 +13544,7 @@
       <c r="A216">
         <v>90776</v>
       </c>
-      <c r="B216" s="2">
+      <c r="B216">
         <f t="shared" si="3"/>
         <v>22461</v>
       </c>
@@ -13606,7 +13604,7 @@
       <c r="A217">
         <v>90876</v>
       </c>
-      <c r="B217" s="2">
+      <c r="B217">
         <f t="shared" si="3"/>
         <v>22561</v>
       </c>
@@ -13666,7 +13664,7 @@
       <c r="A218">
         <v>90979</v>
       </c>
-      <c r="B218" s="2">
+      <c r="B218">
         <f t="shared" si="3"/>
         <v>22664</v>
       </c>
@@ -13726,7 +13724,7 @@
       <c r="A219">
         <v>91082</v>
       </c>
-      <c r="B219" s="2">
+      <c r="B219">
         <f t="shared" si="3"/>
         <v>22767</v>
       </c>
@@ -13786,7 +13784,7 @@
       <c r="A220">
         <v>91189</v>
       </c>
-      <c r="B220" s="2">
+      <c r="B220">
         <f t="shared" si="3"/>
         <v>22874</v>
       </c>
@@ -13846,7 +13844,7 @@
       <c r="A221">
         <v>91294</v>
       </c>
-      <c r="B221" s="2">
+      <c r="B221">
         <f t="shared" si="3"/>
         <v>22979</v>
       </c>
@@ -13906,7 +13904,7 @@
       <c r="A222">
         <v>91401</v>
       </c>
-      <c r="B222" s="2">
+      <c r="B222">
         <f t="shared" si="3"/>
         <v>23086</v>
       </c>
@@ -13966,7 +13964,7 @@
       <c r="A223">
         <v>91507</v>
       </c>
-      <c r="B223" s="2">
+      <c r="B223">
         <f t="shared" si="3"/>
         <v>23192</v>
       </c>
@@ -14026,7 +14024,7 @@
       <c r="A224">
         <v>91613</v>
       </c>
-      <c r="B224" s="2">
+      <c r="B224">
         <f t="shared" si="3"/>
         <v>23298</v>
       </c>
@@ -14086,7 +14084,7 @@
       <c r="A225">
         <v>91720</v>
       </c>
-      <c r="B225" s="2">
+      <c r="B225">
         <f t="shared" si="3"/>
         <v>23405</v>
       </c>
@@ -14146,7 +14144,7 @@
       <c r="A226">
         <v>91826</v>
       </c>
-      <c r="B226" s="2">
+      <c r="B226">
         <f t="shared" si="3"/>
         <v>23511</v>
       </c>
@@ -14206,7 +14204,7 @@
       <c r="A227">
         <v>91932</v>
       </c>
-      <c r="B227" s="2">
+      <c r="B227">
         <f t="shared" si="3"/>
         <v>23617</v>
       </c>
@@ -14266,7 +14264,7 @@
       <c r="A228">
         <v>92039</v>
       </c>
-      <c r="B228" s="2">
+      <c r="B228">
         <f t="shared" si="3"/>
         <v>23724</v>
       </c>
@@ -14326,7 +14324,7 @@
       <c r="A229">
         <v>92143</v>
       </c>
-      <c r="B229" s="2">
+      <c r="B229">
         <f t="shared" si="3"/>
         <v>23828</v>
       </c>
@@ -14386,7 +14384,7 @@
       <c r="A230">
         <v>92248</v>
       </c>
-      <c r="B230" s="2">
+      <c r="B230">
         <f t="shared" si="3"/>
         <v>23933</v>
       </c>
@@ -14446,7 +14444,7 @@
       <c r="A231">
         <v>92350</v>
       </c>
-      <c r="B231" s="2">
+      <c r="B231">
         <f t="shared" si="3"/>
         <v>24035</v>
       </c>
@@ -14506,7 +14504,7 @@
       <c r="A232">
         <v>92455</v>
       </c>
-      <c r="B232" s="2">
+      <c r="B232">
         <f t="shared" si="3"/>
         <v>24140</v>
       </c>
@@ -14566,7 +14564,7 @@
       <c r="A233">
         <v>92561</v>
       </c>
-      <c r="B233" s="2">
+      <c r="B233">
         <f t="shared" si="3"/>
         <v>24246</v>
       </c>
@@ -14626,7 +14624,7 @@
       <c r="A234">
         <v>92665</v>
       </c>
-      <c r="B234" s="2">
+      <c r="B234">
         <f t="shared" si="3"/>
         <v>24350</v>
       </c>
@@ -14686,7 +14684,7 @@
       <c r="A235">
         <v>92773</v>
       </c>
-      <c r="B235" s="2">
+      <c r="B235">
         <f t="shared" si="3"/>
         <v>24458</v>
       </c>
@@ -14746,7 +14744,7 @@
       <c r="A236">
         <v>92879</v>
       </c>
-      <c r="B236" s="2">
+      <c r="B236">
         <f t="shared" si="3"/>
         <v>24564</v>
       </c>
@@ -14806,7 +14804,7 @@
       <c r="A237">
         <v>92987</v>
       </c>
-      <c r="B237" s="2">
+      <c r="B237">
         <f t="shared" si="3"/>
         <v>24672</v>
       </c>
@@ -14866,7 +14864,7 @@
       <c r="A238">
         <v>93095</v>
       </c>
-      <c r="B238" s="2">
+      <c r="B238">
         <f t="shared" si="3"/>
         <v>24780</v>
       </c>
@@ -14926,7 +14924,7 @@
       <c r="A239">
         <v>93203</v>
       </c>
-      <c r="B239" s="2">
+      <c r="B239">
         <f t="shared" si="3"/>
         <v>24888</v>
       </c>
@@ -14986,7 +14984,7 @@
       <c r="A240">
         <v>93312</v>
       </c>
-      <c r="B240" s="2">
+      <c r="B240">
         <f t="shared" si="3"/>
         <v>24997</v>
       </c>
@@ -15046,7 +15044,7 @@
       <c r="A241">
         <v>93419</v>
       </c>
-      <c r="B241" s="2">
+      <c r="B241">
         <f t="shared" si="3"/>
         <v>25104</v>
       </c>
@@ -15106,7 +15104,7 @@
       <c r="A242">
         <v>93526</v>
       </c>
-      <c r="B242" s="2">
+      <c r="B242">
         <f t="shared" si="3"/>
         <v>25211</v>
       </c>
@@ -15166,7 +15164,7 @@
       <c r="A243">
         <v>93632</v>
       </c>
-      <c r="B243" s="2">
+      <c r="B243">
         <f t="shared" si="3"/>
         <v>25317</v>
       </c>
@@ -15226,7 +15224,7 @@
       <c r="A244">
         <v>93737</v>
       </c>
-      <c r="B244" s="2">
+      <c r="B244">
         <f t="shared" si="3"/>
         <v>25422</v>
       </c>
@@ -15286,7 +15284,7 @@
       <c r="A245">
         <v>93844</v>
       </c>
-      <c r="B245" s="2">
+      <c r="B245">
         <f t="shared" si="3"/>
         <v>25529</v>
       </c>
@@ -15346,7 +15344,7 @@
       <c r="A246">
         <v>93948</v>
       </c>
-      <c r="B246" s="2">
+      <c r="B246">
         <f t="shared" si="3"/>
         <v>25633</v>
       </c>
@@ -15406,7 +15404,7 @@
       <c r="A247">
         <v>94054</v>
       </c>
-      <c r="B247" s="2">
+      <c r="B247">
         <f t="shared" si="3"/>
         <v>25739</v>
       </c>
@@ -15466,7 +15464,7 @@
       <c r="A248">
         <v>94159</v>
       </c>
-      <c r="B248" s="2">
+      <c r="B248">
         <f t="shared" si="3"/>
         <v>25844</v>
       </c>
@@ -15526,7 +15524,7 @@
       <c r="A249">
         <v>94266</v>
       </c>
-      <c r="B249" s="2">
+      <c r="B249">
         <f t="shared" si="3"/>
         <v>25951</v>
       </c>
@@ -15586,7 +15584,7 @@
       <c r="A250">
         <v>94373</v>
       </c>
-      <c r="B250" s="2">
+      <c r="B250">
         <f t="shared" si="3"/>
         <v>26058</v>
       </c>
@@ -15646,7 +15644,7 @@
       <c r="A251">
         <v>94480</v>
       </c>
-      <c r="B251" s="2">
+      <c r="B251">
         <f t="shared" si="3"/>
         <v>26165</v>
       </c>
@@ -15706,7 +15704,7 @@
       <c r="A252">
         <v>94587</v>
       </c>
-      <c r="B252" s="2">
+      <c r="B252">
         <f t="shared" si="3"/>
         <v>26272</v>
       </c>
@@ -15766,7 +15764,7 @@
       <c r="A253">
         <v>94695</v>
       </c>
-      <c r="B253" s="2">
+      <c r="B253">
         <f t="shared" si="3"/>
         <v>26380</v>
       </c>
@@ -15826,7 +15824,7 @@
       <c r="A254">
         <v>94801</v>
       </c>
-      <c r="B254" s="2">
+      <c r="B254">
         <f t="shared" si="3"/>
         <v>26486</v>
       </c>
@@ -15886,7 +15884,7 @@
       <c r="A255">
         <v>94909</v>
       </c>
-      <c r="B255" s="2">
+      <c r="B255">
         <f t="shared" si="3"/>
         <v>26594</v>
       </c>
@@ -15946,7 +15944,7 @@
       <c r="A256">
         <v>95015</v>
       </c>
-      <c r="B256" s="2">
+      <c r="B256">
         <f t="shared" si="3"/>
         <v>26700</v>
       </c>
@@ -16006,7 +16004,7 @@
       <c r="A257">
         <v>95124</v>
       </c>
-      <c r="B257" s="2">
+      <c r="B257">
         <f t="shared" si="3"/>
         <v>26809</v>
       </c>
@@ -16066,7 +16064,7 @@
       <c r="A258">
         <v>95233</v>
       </c>
-      <c r="B258" s="2">
+      <c r="B258">
         <f t="shared" si="3"/>
         <v>26918</v>
       </c>
@@ -16126,7 +16124,7 @@
       <c r="A259">
         <v>95339</v>
       </c>
-      <c r="B259" s="2">
+      <c r="B259">
         <f t="shared" si="3"/>
         <v>27024</v>
       </c>
@@ -16186,7 +16184,7 @@
       <c r="A260">
         <v>95448</v>
       </c>
-      <c r="B260" s="2">
+      <c r="B260">
         <f t="shared" si="3"/>
         <v>27133</v>
       </c>
@@ -16246,7 +16244,7 @@
       <c r="A261">
         <v>95554</v>
       </c>
-      <c r="B261" s="2">
+      <c r="B261">
         <f t="shared" ref="B261:B324" si="4">A261-$A$4</f>
         <v>27239</v>
       </c>
@@ -16306,7 +16304,7 @@
       <c r="A262">
         <v>95663</v>
       </c>
-      <c r="B262" s="2">
+      <c r="B262">
         <f t="shared" si="4"/>
         <v>27348</v>
       </c>
@@ -16366,7 +16364,7 @@
       <c r="A263">
         <v>95769</v>
       </c>
-      <c r="B263" s="2">
+      <c r="B263">
         <f t="shared" si="4"/>
         <v>27454</v>
       </c>
@@ -16426,7 +16424,7 @@
       <c r="A264">
         <v>95875</v>
       </c>
-      <c r="B264" s="2">
+      <c r="B264">
         <f t="shared" si="4"/>
         <v>27560</v>
       </c>
@@ -16486,7 +16484,7 @@
       <c r="A265">
         <v>95979</v>
       </c>
-      <c r="B265" s="2">
+      <c r="B265">
         <f t="shared" si="4"/>
         <v>27664</v>
       </c>
@@ -16546,7 +16544,7 @@
       <c r="A266">
         <v>96081</v>
       </c>
-      <c r="B266" s="2">
+      <c r="B266">
         <f t="shared" si="4"/>
         <v>27766</v>
       </c>
@@ -16606,7 +16604,7 @@
       <c r="A267">
         <v>96187</v>
       </c>
-      <c r="B267" s="2">
+      <c r="B267">
         <f t="shared" si="4"/>
         <v>27872</v>
       </c>
@@ -16666,7 +16664,7 @@
       <c r="A268">
         <v>96291</v>
       </c>
-      <c r="B268" s="2">
+      <c r="B268">
         <f t="shared" si="4"/>
         <v>27976</v>
       </c>
@@ -16726,7 +16724,7 @@
       <c r="A269">
         <v>96394</v>
       </c>
-      <c r="B269" s="2">
+      <c r="B269">
         <f t="shared" si="4"/>
         <v>28079</v>
       </c>
@@ -16786,7 +16784,7 @@
       <c r="A270">
         <v>96497</v>
       </c>
-      <c r="B270" s="2">
+      <c r="B270">
         <f t="shared" si="4"/>
         <v>28182</v>
       </c>
@@ -16846,7 +16844,7 @@
       <c r="A271">
         <v>96601</v>
       </c>
-      <c r="B271" s="2">
+      <c r="B271">
         <f t="shared" si="4"/>
         <v>28286</v>
       </c>
@@ -16906,7 +16904,7 @@
       <c r="A272">
         <v>96705</v>
       </c>
-      <c r="B272" s="2">
+      <c r="B272">
         <f t="shared" si="4"/>
         <v>28390</v>
       </c>
@@ -16966,7 +16964,7 @@
       <c r="A273">
         <v>96809</v>
       </c>
-      <c r="B273" s="2">
+      <c r="B273">
         <f t="shared" si="4"/>
         <v>28494</v>
       </c>
@@ -17026,7 +17024,7 @@
       <c r="A274">
         <v>96915</v>
       </c>
-      <c r="B274" s="2">
+      <c r="B274">
         <f t="shared" si="4"/>
         <v>28600</v>
       </c>
@@ -17086,7 +17084,7 @@
       <c r="A275">
         <v>97020</v>
       </c>
-      <c r="B275" s="2">
+      <c r="B275">
         <f t="shared" si="4"/>
         <v>28705</v>
       </c>
@@ -17146,7 +17144,7 @@
       <c r="A276">
         <v>97126</v>
       </c>
-      <c r="B276" s="2">
+      <c r="B276">
         <f t="shared" si="4"/>
         <v>28811</v>
       </c>
@@ -17206,7 +17204,7 @@
       <c r="A277">
         <v>97231</v>
       </c>
-      <c r="B277" s="2">
+      <c r="B277">
         <f t="shared" si="4"/>
         <v>28916</v>
       </c>
@@ -17266,7 +17264,7 @@
       <c r="A278">
         <v>97337</v>
       </c>
-      <c r="B278" s="2">
+      <c r="B278">
         <f t="shared" si="4"/>
         <v>29022</v>
       </c>
@@ -17326,7 +17324,7 @@
       <c r="A279">
         <v>97442</v>
       </c>
-      <c r="B279" s="2">
+      <c r="B279">
         <f t="shared" si="4"/>
         <v>29127</v>
       </c>
@@ -17386,7 +17384,7 @@
       <c r="A280">
         <v>97547</v>
       </c>
-      <c r="B280" s="2">
+      <c r="B280">
         <f t="shared" si="4"/>
         <v>29232</v>
       </c>
@@ -17446,7 +17444,7 @@
       <c r="A281">
         <v>97653</v>
       </c>
-      <c r="B281" s="2">
+      <c r="B281">
         <f t="shared" si="4"/>
         <v>29338</v>
       </c>
@@ -17506,7 +17504,7 @@
       <c r="A282">
         <v>97760</v>
       </c>
-      <c r="B282" s="2">
+      <c r="B282">
         <f t="shared" si="4"/>
         <v>29445</v>
       </c>
@@ -17566,7 +17564,7 @@
       <c r="A283">
         <v>97865</v>
       </c>
-      <c r="B283" s="2">
+      <c r="B283">
         <f t="shared" si="4"/>
         <v>29550</v>
       </c>
@@ -17626,7 +17624,7 @@
       <c r="A284">
         <v>97971</v>
       </c>
-      <c r="B284" s="2">
+      <c r="B284">
         <f t="shared" si="4"/>
         <v>29656</v>
       </c>
@@ -17686,7 +17684,7 @@
       <c r="A285">
         <v>98074</v>
       </c>
-      <c r="B285" s="2">
+      <c r="B285">
         <f t="shared" si="4"/>
         <v>29759</v>
       </c>
@@ -17746,7 +17744,7 @@
       <c r="A286">
         <v>98179</v>
       </c>
-      <c r="B286" s="2">
+      <c r="B286">
         <f t="shared" si="4"/>
         <v>29864</v>
       </c>
@@ -17806,7 +17804,7 @@
       <c r="A287">
         <v>98283</v>
       </c>
-      <c r="B287" s="2">
+      <c r="B287">
         <f t="shared" si="4"/>
         <v>29968</v>
       </c>
@@ -17866,7 +17864,7 @@
       <c r="A288">
         <v>98390</v>
       </c>
-      <c r="B288" s="2">
+      <c r="B288">
         <f t="shared" si="4"/>
         <v>30075</v>
       </c>
@@ -17926,7 +17924,7 @@
       <c r="A289">
         <v>98497</v>
       </c>
-      <c r="B289" s="2">
+      <c r="B289">
         <f t="shared" si="4"/>
         <v>30182</v>
       </c>
@@ -17986,7 +17984,7 @@
       <c r="A290">
         <v>98603</v>
       </c>
-      <c r="B290" s="2">
+      <c r="B290">
         <f t="shared" si="4"/>
         <v>30288</v>
       </c>
@@ -18046,7 +18044,7 @@
       <c r="A291">
         <v>98710</v>
       </c>
-      <c r="B291" s="2">
+      <c r="B291">
         <f t="shared" si="4"/>
         <v>30395</v>
       </c>
@@ -18106,7 +18104,7 @@
       <c r="A292">
         <v>98816</v>
       </c>
-      <c r="B292" s="2">
+      <c r="B292">
         <f t="shared" si="4"/>
         <v>30501</v>
       </c>
@@ -18166,7 +18164,7 @@
       <c r="A293">
         <v>98924</v>
       </c>
-      <c r="B293" s="2">
+      <c r="B293">
         <f t="shared" si="4"/>
         <v>30609</v>
       </c>
@@ -18226,7 +18224,7 @@
       <c r="A294">
         <v>99032</v>
       </c>
-      <c r="B294" s="2">
+      <c r="B294">
         <f t="shared" si="4"/>
         <v>30717</v>
       </c>
@@ -18286,7 +18284,7 @@
       <c r="A295">
         <v>99138</v>
       </c>
-      <c r="B295" s="2">
+      <c r="B295">
         <f t="shared" si="4"/>
         <v>30823</v>
       </c>
@@ -18346,7 +18344,7 @@
       <c r="A296">
         <v>99246</v>
       </c>
-      <c r="B296" s="2">
+      <c r="B296">
         <f t="shared" si="4"/>
         <v>30931</v>
       </c>
@@ -18406,7 +18404,7 @@
       <c r="A297">
         <v>99353</v>
       </c>
-      <c r="B297" s="2">
+      <c r="B297">
         <f t="shared" si="4"/>
         <v>31038</v>
       </c>
@@ -18466,7 +18464,7 @@
       <c r="A298">
         <v>99459</v>
       </c>
-      <c r="B298" s="2">
+      <c r="B298">
         <f t="shared" si="4"/>
         <v>31144</v>
       </c>
@@ -18526,7 +18524,7 @@
       <c r="A299">
         <v>99565</v>
       </c>
-      <c r="B299" s="2">
+      <c r="B299">
         <f t="shared" si="4"/>
         <v>31250</v>
       </c>
@@ -18586,7 +18584,7 @@
       <c r="A300">
         <v>99671</v>
       </c>
-      <c r="B300" s="2">
+      <c r="B300">
         <f t="shared" si="4"/>
         <v>31356</v>
       </c>
@@ -18646,7 +18644,7 @@
       <c r="A301">
         <v>99777</v>
       </c>
-      <c r="B301" s="2">
+      <c r="B301">
         <f t="shared" si="4"/>
         <v>31462</v>
       </c>
@@ -18706,7 +18704,7 @@
       <c r="A302">
         <v>99884</v>
       </c>
-      <c r="B302" s="2">
+      <c r="B302">
         <f t="shared" si="4"/>
         <v>31569</v>
       </c>
@@ -18766,7 +18764,7 @@
       <c r="A303">
         <v>99990</v>
       </c>
-      <c r="B303" s="2">
+      <c r="B303">
         <f t="shared" si="4"/>
         <v>31675</v>
       </c>
@@ -18826,7 +18824,7 @@
       <c r="A304">
         <v>100098</v>
       </c>
-      <c r="B304" s="2">
+      <c r="B304">
         <f t="shared" si="4"/>
         <v>31783</v>
       </c>
@@ -18886,7 +18884,7 @@
       <c r="A305">
         <v>100205</v>
       </c>
-      <c r="B305" s="2">
+      <c r="B305">
         <f t="shared" si="4"/>
         <v>31890</v>
       </c>
@@ -18946,7 +18944,7 @@
       <c r="A306">
         <v>100314</v>
       </c>
-      <c r="B306" s="2">
+      <c r="B306">
         <f t="shared" si="4"/>
         <v>31999</v>
       </c>
@@ -19006,7 +19004,7 @@
       <c r="A307">
         <v>100422</v>
       </c>
-      <c r="B307" s="2">
+      <c r="B307">
         <f t="shared" si="4"/>
         <v>32107</v>
       </c>
@@ -19066,7 +19064,7 @@
       <c r="A308">
         <v>100530</v>
       </c>
-      <c r="B308" s="2">
+      <c r="B308">
         <f t="shared" si="4"/>
         <v>32215</v>
       </c>
@@ -19126,7 +19124,7 @@
       <c r="A309">
         <v>100638</v>
       </c>
-      <c r="B309" s="2">
+      <c r="B309">
         <f t="shared" si="4"/>
         <v>32323</v>
       </c>
@@ -19186,7 +19184,7 @@
       <c r="A310">
         <v>100746</v>
       </c>
-      <c r="B310" s="2">
+      <c r="B310">
         <f t="shared" si="4"/>
         <v>32431</v>
       </c>
@@ -19246,7 +19244,7 @@
       <c r="A311">
         <v>100853</v>
       </c>
-      <c r="B311" s="2">
+      <c r="B311">
         <f t="shared" si="4"/>
         <v>32538</v>
       </c>
@@ -19306,7 +19304,7 @@
       <c r="A312">
         <v>100962</v>
       </c>
-      <c r="B312" s="2">
+      <c r="B312">
         <f t="shared" si="4"/>
         <v>32647</v>
       </c>
@@ -19366,7 +19364,7 @@
       <c r="A313">
         <v>101069</v>
       </c>
-      <c r="B313" s="2">
+      <c r="B313">
         <f t="shared" si="4"/>
         <v>32754</v>
       </c>
@@ -19426,7 +19424,7 @@
       <c r="A314">
         <v>101178</v>
       </c>
-      <c r="B314" s="2">
+      <c r="B314">
         <f t="shared" si="4"/>
         <v>32863</v>
       </c>
@@ -19486,7 +19484,7 @@
       <c r="A315">
         <v>101287</v>
       </c>
-      <c r="B315" s="2">
+      <c r="B315">
         <f t="shared" si="4"/>
         <v>32972</v>
       </c>
@@ -19546,7 +19544,7 @@
       <c r="A316">
         <v>101396</v>
       </c>
-      <c r="B316" s="2">
+      <c r="B316">
         <f t="shared" si="4"/>
         <v>33081</v>
       </c>
@@ -19606,7 +19604,7 @@
       <c r="A317">
         <v>101506</v>
       </c>
-      <c r="B317" s="2">
+      <c r="B317">
         <f t="shared" si="4"/>
         <v>33191</v>
       </c>
@@ -19666,7 +19664,7 @@
       <c r="A318">
         <v>101616</v>
       </c>
-      <c r="B318" s="2">
+      <c r="B318">
         <f t="shared" si="4"/>
         <v>33301</v>
       </c>
@@ -19726,7 +19724,7 @@
       <c r="A319">
         <v>101724</v>
       </c>
-      <c r="B319" s="2">
+      <c r="B319">
         <f t="shared" si="4"/>
         <v>33409</v>
       </c>
@@ -19786,7 +19784,7 @@
       <c r="A320">
         <v>101831</v>
       </c>
-      <c r="B320" s="2">
+      <c r="B320">
         <f t="shared" si="4"/>
         <v>33516</v>
       </c>
@@ -19846,7 +19844,7 @@
       <c r="A321">
         <v>101938</v>
       </c>
-      <c r="B321" s="2">
+      <c r="B321">
         <f t="shared" si="4"/>
         <v>33623</v>
       </c>
@@ -19906,7 +19904,7 @@
       <c r="A322">
         <v>102044</v>
       </c>
-      <c r="B322" s="2">
+      <c r="B322">
         <f t="shared" si="4"/>
         <v>33729</v>
       </c>
@@ -19966,7 +19964,7 @@
       <c r="A323">
         <v>102150</v>
       </c>
-      <c r="B323" s="2">
+      <c r="B323">
         <f t="shared" si="4"/>
         <v>33835</v>
       </c>
@@ -20026,7 +20024,7 @@
       <c r="A324">
         <v>102253</v>
       </c>
-      <c r="B324" s="2">
+      <c r="B324">
         <f t="shared" si="4"/>
         <v>33938</v>
       </c>
@@ -20086,7 +20084,7 @@
       <c r="A325">
         <v>102359</v>
       </c>
-      <c r="B325" s="2">
+      <c r="B325">
         <f t="shared" ref="B325:B342" si="5">A325-$A$4</f>
         <v>34044</v>
       </c>
@@ -20146,7 +20144,7 @@
       <c r="A326">
         <v>102463</v>
       </c>
-      <c r="B326" s="2">
+      <c r="B326">
         <f t="shared" si="5"/>
         <v>34148</v>
       </c>
@@ -20206,7 +20204,7 @@
       <c r="A327">
         <v>102568</v>
       </c>
-      <c r="B327" s="2">
+      <c r="B327">
         <f t="shared" si="5"/>
         <v>34253</v>
       </c>
@@ -20266,7 +20264,7 @@
       <c r="A328">
         <v>102674</v>
       </c>
-      <c r="B328" s="2">
+      <c r="B328">
         <f t="shared" si="5"/>
         <v>34359</v>
       </c>
@@ -20326,7 +20324,7 @@
       <c r="A329">
         <v>102781</v>
       </c>
-      <c r="B329" s="2">
+      <c r="B329">
         <f t="shared" si="5"/>
         <v>34466</v>
       </c>
@@ -20386,7 +20384,7 @@
       <c r="A330">
         <v>102889</v>
       </c>
-      <c r="B330" s="2">
+      <c r="B330">
         <f t="shared" si="5"/>
         <v>34574</v>
       </c>
@@ -20446,7 +20444,7 @@
       <c r="A331">
         <v>102994</v>
       </c>
-      <c r="B331" s="2">
+      <c r="B331">
         <f t="shared" si="5"/>
         <v>34679</v>
       </c>
@@ -20506,7 +20504,7 @@
       <c r="A332">
         <v>103101</v>
       </c>
-      <c r="B332" s="2">
+      <c r="B332">
         <f t="shared" si="5"/>
         <v>34786</v>
       </c>
@@ -20566,7 +20564,7 @@
       <c r="A333">
         <v>103207</v>
       </c>
-      <c r="B333" s="2">
+      <c r="B333">
         <f t="shared" si="5"/>
         <v>34892</v>
       </c>
@@ -20626,7 +20624,7 @@
       <c r="A334">
         <v>103314</v>
       </c>
-      <c r="B334" s="2">
+      <c r="B334">
         <f t="shared" si="5"/>
         <v>34999</v>
       </c>
@@ -20686,7 +20684,7 @@
       <c r="A335">
         <v>103421</v>
       </c>
-      <c r="B335" s="2">
+      <c r="B335">
         <f t="shared" si="5"/>
         <v>35106</v>
       </c>
@@ -20746,7 +20744,7 @@
       <c r="A336">
         <v>103527</v>
       </c>
-      <c r="B336" s="2">
+      <c r="B336">
         <f t="shared" si="5"/>
         <v>35212</v>
       </c>
@@ -20806,7 +20804,7 @@
       <c r="A337">
         <v>103635</v>
       </c>
-      <c r="B337" s="2">
+      <c r="B337">
         <f t="shared" si="5"/>
         <v>35320</v>
       </c>
@@ -20866,7 +20864,7 @@
       <c r="A338">
         <v>103741</v>
       </c>
-      <c r="B338" s="2">
+      <c r="B338">
         <f t="shared" si="5"/>
         <v>35426</v>
       </c>
@@ -20926,7 +20924,7 @@
       <c r="A339">
         <v>103846</v>
       </c>
-      <c r="B339" s="2">
+      <c r="B339">
         <f t="shared" si="5"/>
         <v>35531</v>
       </c>
@@ -20986,7 +20984,7 @@
       <c r="A340">
         <v>103952</v>
       </c>
-      <c r="B340" s="2">
+      <c r="B340">
         <f t="shared" si="5"/>
         <v>35637</v>
       </c>
@@ -21046,7 +21044,7 @@
       <c r="A341">
         <v>104057</v>
       </c>
-      <c r="B341" s="2">
+      <c r="B341">
         <f t="shared" si="5"/>
         <v>35742</v>
       </c>
@@ -21106,7 +21104,7 @@
       <c r="A342">
         <v>104165</v>
       </c>
-      <c r="B342" s="2">
+      <c r="B342">
         <f t="shared" si="5"/>
         <v>35850</v>
       </c>
@@ -21123,9 +21121,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="11">
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
@@ -21134,6 +21129,9 @@
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:S1"/>
     <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>